<commit_message>
I made changes to the excel file
</commit_message>
<xml_diff>
--- a/qmbe 3710.xlsx
+++ b/qmbe 3710.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodge\OneDrive\Desktop\QMBE_3730_Kennedy_Odongo_2025\QMBE_3730_Kennedy_Odongo_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73EFE4E1-D257-4F23-94F6-DC42EBD419FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826C44B2-4E4F-4D57-B211-D2920C8FDF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{A20CB50A-E041-4AF7-9794-71EF0759D609}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>hswgdhedgfsd</t>
+  </si>
+  <si>
+    <t>ljfwheuodgahfdlkgjdf;kgkj</t>
   </si>
 </sst>
 </file>
@@ -410,15 +413,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282E2F80-44C5-4448-ACC1-C66649ADA8C7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>